<commit_message>
Added module 4 exercises
</commit_message>
<xml_diff>
--- a/Module 4/3- Scenarios/Decisions - Scenarios.xlsx
+++ b/Module 4/3- Scenarios/Decisions - Scenarios.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianca.dragu\Documents\UiPath\Switch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edmun\Desktop\SCS-3757-Robotic-and-Intelligent-Process-Automation\Module 4\3- Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D63DA01A-ECA6-47E8-8C58-07C7409B8652}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17004" yWindow="-17388" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17010" yWindow="-17385" windowWidth="30930" windowHeight="16890"/>
   </bookViews>
   <sheets>
     <sheet name="20191115" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>Transaction Type</t>
   </si>
@@ -111,14 +110,17 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>Transaction has been processed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -605,8 +607,8 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -659,33 +661,33 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <numFmt numFmtId="10" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="10" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="10" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="10" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="10" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="10" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="10" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -702,19 +704,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Decisions" displayName="Decisions" ref="A1:J9" totalsRowShown="0">
-  <autoFilter ref="A1:J9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Decisions" displayName="Decisions" ref="A1:J9" totalsRowShown="0">
+  <autoFilter ref="A1:J9"/>
   <tableColumns count="10">
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Transaction Type"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Cash In" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="On Us Check" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Not On US Check" dataDxfId="5"/>
-    <tableColumn id="1" xr3:uid="{39D81A04-7CAF-4B00-AC2B-735BB8EFA825}" name="Check #1" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{98F4943B-E0A3-434F-94EE-AA91055786B1}" name="Check #2" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{4B10E16B-6684-4754-8EBF-AA8AF93404D6}" name="Transaction #" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{D56D6A53-BC2C-4104-9CE2-E3450CB1090F}" name="First Name" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Last Name"/>
-    <tableColumn id="10" xr3:uid="{C5FE1E98-B665-4C86-AE42-6398A64E240C}" name="Comment" dataDxfId="0"/>
+    <tableColumn id="3" name="Transaction Type"/>
+    <tableColumn id="4" name="Cash In" dataDxfId="7"/>
+    <tableColumn id="5" name="On Us Check" dataDxfId="6"/>
+    <tableColumn id="6" name="Not On US Check" dataDxfId="5"/>
+    <tableColumn id="1" name="Check #1" dataDxfId="4"/>
+    <tableColumn id="2" name="Check #2" dataDxfId="3"/>
+    <tableColumn id="12" name="Transaction #" dataDxfId="2"/>
+    <tableColumn id="11" name="First Name" dataDxfId="1"/>
+    <tableColumn id="7" name="Last Name"/>
+    <tableColumn id="10" name="Comment" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1016,24 +1018,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" customWidth="1"/>
-    <col min="4" max="8" width="17.21875" customWidth="1"/>
-    <col min="9" max="9" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.77734375" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="8" width="17.28515625" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1065,7 +1067,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1080,7 +1082,9 @@
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3">
+        <v>732837</v>
+      </c>
       <c r="H2" t="s">
         <v>4</v>
       </c>
@@ -1089,7 +1093,7 @@
       </c>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1102,7 +1106,9 @@
       <c r="F3" s="2">
         <v>160.08000000000001</v>
       </c>
-      <c r="G3" s="3"/>
+      <c r="G3" s="3">
+        <v>717203</v>
+      </c>
       <c r="H3" t="s">
         <v>7</v>
       </c>
@@ -1111,7 +1117,7 @@
       </c>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1139,7 +1145,7 @@
       </c>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1163,9 +1169,11 @@
       <c r="I5" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="1"/>
+      <c r="J5" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1178,7 +1186,9 @@
       <c r="F6" s="2">
         <v>34.270000000000003</v>
       </c>
-      <c r="G6" s="3"/>
+      <c r="G6" s="3">
+        <v>717203</v>
+      </c>
       <c r="H6" t="s">
         <v>11</v>
       </c>
@@ -1187,7 +1197,7 @@
       </c>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1202,7 +1212,9 @@
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="3"/>
+      <c r="G7" s="3">
+        <v>732838</v>
+      </c>
       <c r="H7" t="s">
         <v>13</v>
       </c>
@@ -1211,7 +1223,7 @@
       </c>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1226,7 +1238,9 @@
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="3"/>
+      <c r="G8" s="3">
+        <v>717203</v>
+      </c>
       <c r="H8" t="s">
         <v>15</v>
       </c>
@@ -1235,7 +1249,7 @@
       </c>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1477,6 +1491,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1485,20 +1505,38 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{522BCE10-EF20-4CE7-9DCF-6978E2837A0C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{522BCE10-EF20-4CE7-9DCF-6978E2837A0C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="911b8362-47a7-4e55-be9b-e7010cb44337"/>
+    <ds:schemaRef ds:uri="e65b6849-a419-4724-a870-b3d895c8345c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8143AC49-7F69-4C96-9550-CE71E95D751C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F95DC0C5-3A65-4895-8F87-13E6F72BF9B2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F95DC0C5-3A65-4895-8F87-13E6F72BF9B2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8143AC49-7F69-4C96-9550-CE71E95D751C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>